<commit_message>
commit com a aula 02
</commit_message>
<xml_diff>
--- a/acoes_pura.xlsx
+++ b/acoes_pura.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{B30F972A-2396-4A81-B421-5385D6EF7650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="6_{B30F972A-2396-4A81-B421-5385D6EF7650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70C78A25-7A47-4350-84FA-7D47EB7B343F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
-    <sheet name="Total_de_acoes" sheetId="2" r:id="rId2"/>
-    <sheet name="Ticker" sheetId="3" r:id="rId3"/>
+    <sheet name="ChatGPT" sheetId="4" r:id="rId2"/>
+    <sheet name="Total_de_acoes" sheetId="2" r:id="rId3"/>
+    <sheet name="Ticker" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="1011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="1051">
   <si>
     <t>Ativo</t>
   </si>
@@ -3050,13 +3051,133 @@
   </si>
   <si>
     <t>Minasmáquinas</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Segmento</t>
+  </si>
+  <si>
+    <t>Idade (anos)</t>
+  </si>
+  <si>
+    <t>Petróleo</t>
+  </si>
+  <si>
+    <t>Saúde</t>
+  </si>
+  <si>
+    <t>Moda</t>
+  </si>
+  <si>
+    <t>Alimentos</t>
+  </si>
+  <si>
+    <t>Varejo</t>
+  </si>
+  <si>
+    <t>Transporte Aéreo</t>
+  </si>
+  <si>
+    <t>Finanças</t>
+  </si>
+  <si>
+    <t>Financeiro</t>
+  </si>
+  <si>
+    <t>Seguros</t>
+  </si>
+  <si>
+    <t>Química</t>
+  </si>
+  <si>
+    <t>Energia</t>
+  </si>
+  <si>
+    <t>FinTech</t>
+  </si>
+  <si>
+    <t>Educação</t>
+  </si>
+  <si>
+    <t>Mineração</t>
+  </si>
+  <si>
+    <t>Viagens</t>
+  </si>
+  <si>
+    <t>Construção</t>
+  </si>
+  <si>
+    <t>Metalurgia</t>
+  </si>
+  <si>
+    <t>Aeroespacial</t>
+  </si>
+  <si>
+    <t>Siderurgia</t>
+  </si>
+  <si>
+    <t>Logística</t>
+  </si>
+  <si>
+    <t>Farmacêutico</t>
+  </si>
+  <si>
+    <t>Aluguel de carros</t>
+  </si>
+  <si>
+    <t>Tecnologia</t>
+  </si>
+  <si>
+    <t>Imobiliário</t>
+  </si>
+  <si>
+    <t>Cosméticos</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Saneamento Básico</t>
+  </si>
+  <si>
+    <t>Agronegócio</t>
+  </si>
+  <si>
+    <t>Papel e Celulose</t>
+  </si>
+  <si>
+    <t>Telecomunicações</t>
+  </si>
+  <si>
+    <t>TONS</t>
+  </si>
+  <si>
+    <t>Serviços Financeiros</t>
+  </si>
+  <si>
+    <t>Energia Elétrica</t>
+  </si>
+  <si>
+    <t>Petróleo e Gás</t>
+  </si>
+  <si>
+    <t>Urapar</t>
+  </si>
+  <si>
+    <t>Viva</t>
+  </si>
+  <si>
+    <t>Engenharia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3092,6 +3213,21 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -3119,7 +3255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3127,11 +3263,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3162,11 +3313,54 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3177,6 +3371,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3382,7 +3580,7 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -18208,6 +18406,968 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1950EE-83F4-4939-8A56-244CC6A3B075}">
+  <dimension ref="A1:C85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="18" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C2" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C3" s="19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C4" s="19">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C5" s="19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C6" s="19">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C7" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C8" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C9" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C10" s="19">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C11" s="19">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C12" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C13" s="19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C14" s="19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C15" s="19">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C16" s="19">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C17" s="19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C18" s="19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C19" s="19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C20" s="19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C21" s="19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C22" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C23" s="19">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C24" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C25" s="19">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C26" s="19">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C27" s="19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C28" s="19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C29" s="19">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C30" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C31" s="19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C32" s="19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C33" s="19">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C34" s="19">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C35" s="19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C36" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C37" s="19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C38" s="19">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C39" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C40" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C41" s="19">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C42" s="19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C43" s="19">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C44" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C45" s="19">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C46" s="19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C47" s="19">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C48" s="19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C49" s="19">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C50" s="19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C51" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C52" s="19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C53" s="19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C54" s="19">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C55" s="19">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C56" s="19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C57" s="19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C58" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C59" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C60" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C61" s="19">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C62" s="21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C63" s="19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C64" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C65" s="21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C66" s="21">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C67" s="21">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C68" s="19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C69" s="19">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C70" s="19">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C71" s="19">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="20" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C72" s="21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C73" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C74" s="21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C75" s="21">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="20" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B76" s="20" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C76" s="21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C77" s="19">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C78" s="21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C79" s="19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C80" s="21">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C81" s="21">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="13.8" thickBot="1">
+      <c r="A82" s="20" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C82" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="13.8" thickBot="1">
+      <c r="A83" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C83" s="22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="13.8" thickBot="1">
+      <c r="A84" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C84" s="22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="13.8" thickBot="1">
+      <c r="A85" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C85" s="22">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:C1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -22588,7 +23748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>